<commit_message>
imp ws unidad1 completo
</commit_message>
<xml_diff>
--- a/_DOCs/webserviseV3-1.xlsx
+++ b/_DOCs/webserviseV3-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Confe2\_DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E0AF96-8DED-456E-95E7-C8A28D59214B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA42B381-35E9-461F-980E-34082114FEA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="150">
   <si>
     <t>-</t>
   </si>
@@ -376,9 +376,6 @@
     <t>sexo</t>
   </si>
   <si>
-    <t>masc/fem</t>
-  </si>
-  <si>
     <t>r04testimoniochllenge</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>emociones</t>
+  </si>
+  <si>
+    <t>m/f</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081A2071-6B82-4DF7-B58A-E6A87EDE448E}">
   <dimension ref="B5:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,9 +1119,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
-      <c r="C7" s="7" t="s">
-        <v>94</v>
-      </c>
+      <c r="C7" s="7"/>
       <c r="D7" s="26" t="s">
         <v>17</v>
       </c>
@@ -1351,7 +1349,7 @@
         <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
@@ -1370,13 +1368,13 @@
         <v>14</v>
       </c>
       <c r="F36" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="H36" t="s">
         <v>139</v>
-      </c>
-      <c r="H36" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
@@ -1384,10 +1382,10 @@
         <v>96</v>
       </c>
       <c r="F37" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" t="s">
         <v>148</v>
-      </c>
-      <c r="G37" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
@@ -1542,7 +1540,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="12"/>
     <col min="2" max="2" width="24" style="11" customWidth="1"/>
@@ -1553,7 +1551,7 @@
     <col min="8" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
@@ -1561,7 +1559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>81</v>
       </c>
@@ -1584,12 +1582,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>36</v>
@@ -1604,12 +1602,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>35</v>
@@ -1625,12 +1623,12 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>26</v>
@@ -1645,7 +1643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>4</v>
       </c>
@@ -1665,12 +1663,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>28</v>
@@ -1685,12 +1683,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>29</v>
@@ -1708,12 +1706,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>37</v>
@@ -1731,12 +1729,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>34</v>
@@ -1748,12 +1746,12 @@
       <c r="F11" s="20"/>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>30</v>
@@ -1768,12 +1766,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>38</v>
@@ -1789,12 +1787,12 @@
       </c>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>39</v>
@@ -1812,12 +1810,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>41</v>
@@ -1835,12 +1833,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>43</v>
@@ -1858,12 +1856,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>45</v>
@@ -1881,12 +1879,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>47</v>
@@ -1902,12 +1900,12 @@
       </c>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>48</v>
@@ -1925,12 +1923,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>49</v>
@@ -1948,12 +1946,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>51</v>
@@ -1969,12 +1967,12 @@
       </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>52</v>
@@ -1992,12 +1990,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>54</v>
@@ -2015,12 +2013,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>56</v>
@@ -2038,12 +2036,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>22</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>58</v>
@@ -2061,12 +2059,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>23</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>60</v>
@@ -2084,12 +2082,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>24</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>61</v>
@@ -2107,12 +2105,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>25</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>64</v>
@@ -2130,12 +2128,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>26</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>66</v>
@@ -2153,12 +2151,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>27</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>68</v>
@@ -2176,12 +2174,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>28</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>70</v>
@@ -2199,12 +2197,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>29</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>71</v>
@@ -2222,12 +2220,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>30</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>73</v>
@@ -2243,12 +2241,12 @@
       </c>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>31</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>75</v>
@@ -2264,12 +2262,12 @@
       </c>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>32</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>76</v>
@@ -2285,12 +2283,12 @@
       </c>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>33</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>77</v>
@@ -2305,12 +2303,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>34</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>78</v>

</xml_diff>